<commit_message>
Delay in Message recieved
</commit_message>
<xml_diff>
--- a/data/Trading_Timing.xlsx
+++ b/data/Trading_Timing.xlsx
@@ -8,51 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/eh1618_ic_ac_uk/Documents/Work/Fourth Year/Project/Research/crypto_arbitrage_bot/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="8_{769A6293-BE9D-4368-9A26-58A20B88CFD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FA90E000-7B40-43DB-A72F-5AD6F433FFFC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_01C5BCB9050AE5A40669F7098345844074F78D79" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="23790" yWindow="8540" windowWidth="7500" windowHeight="6000" xr2:uid="{86CF4D6E-8EBA-483F-8F21-1617C54ACE6B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Binance Timing" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t xml:space="preserve">Whole System Before </t>
-  </si>
-  <si>
-    <t>Timestamp on route</t>
-  </si>
-  <si>
-    <t>Whole System After</t>
-  </si>
-  <si>
-    <t>Duration of Arb Finding</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="[hh]:mm:ss"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -82,9 +54,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,37 +373,951 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40706691-1862-4D22-A6E6-3BC3EACB7080}">
-  <dimension ref="A1:D1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A4:D371"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.26953125" customWidth="1"/>
-    <col min="2" max="2" width="20.26953125" customWidth="1"/>
-    <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="22.453125" customWidth="1"/>
+    <col min="1" max="1" width="18.26953125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.26953125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.453125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" s="3"/>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" s="3"/>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" s="2"/>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" s="3"/>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" s="2"/>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" s="3"/>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" s="3"/>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13" s="2"/>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14" s="3"/>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A15" s="2"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" s="3"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" s="3"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" s="2"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" s="3"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" s="2"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" s="3"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A26" s="3"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27" s="2"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A28" s="3"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A29" s="2"/>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A32" s="3"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A33" s="3"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34" s="2"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A35" s="3"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36" s="2"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A39" s="3"/>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A40" s="3"/>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A41" s="2"/>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A42" s="3"/>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A43" s="2"/>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A46" s="3"/>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A47" s="3"/>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A48" s="2"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A49" s="3"/>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A50" s="2"/>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A53" s="3"/>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A54" s="3"/>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A55" s="2"/>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A56" s="3"/>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A57" s="2"/>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A60" s="3"/>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A61" s="3"/>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A62" s="2"/>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A63" s="3"/>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A64" s="2"/>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A67" s="3"/>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A68" s="3"/>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A69" s="2"/>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A70" s="3"/>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A71" s="2"/>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A74" s="3"/>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A75" s="3"/>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A76" s="2"/>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A77" s="3"/>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A78" s="2"/>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A81" s="3"/>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A82" s="3"/>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A83" s="2"/>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A84" s="3"/>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A85" s="2"/>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A88" s="3"/>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A89" s="3"/>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A90" s="2"/>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A91" s="3"/>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A92" s="2"/>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A95" s="3"/>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A96" s="3"/>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A97" s="2"/>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A98" s="3"/>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A99" s="2"/>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A102" s="3"/>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A103" s="3"/>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A104" s="2"/>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A105" s="3"/>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A106" s="2"/>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A109" s="3"/>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A110" s="3"/>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A111" s="2"/>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A112" s="3"/>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A113" s="2"/>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A116" s="3"/>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A117" s="3"/>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A118" s="2"/>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A119" s="3"/>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A120" s="2"/>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A123" s="3"/>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A124" s="3"/>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A125" s="2"/>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A126" s="3"/>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A127" s="2"/>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A130" s="3"/>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A131" s="3"/>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A132" s="2"/>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A133" s="3"/>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A134" s="2"/>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A137" s="3"/>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A138" s="3"/>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A139" s="2"/>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A140" s="3"/>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A141" s="2"/>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A144" s="3"/>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A145" s="3"/>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A146" s="2"/>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A147" s="3"/>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A148" s="2"/>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A151" s="3"/>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A152" s="3"/>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A153" s="2"/>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A154" s="3"/>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A155" s="2"/>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A158" s="3"/>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A159" s="3"/>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A160" s="2"/>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A161" s="3"/>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A162" s="2"/>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A165" s="3"/>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A166" s="3"/>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A167" s="2"/>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A168" s="3"/>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A169" s="2"/>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A172" s="3"/>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A173" s="3"/>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A174" s="2"/>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A175" s="3"/>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A176" s="2"/>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A179" s="3"/>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A180" s="3"/>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A181" s="2"/>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A182" s="3"/>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A183" s="2"/>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A186" s="3"/>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A187" s="3"/>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A188" s="2"/>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A189" s="3"/>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A190" s="2"/>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A193" s="3"/>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A194" s="3"/>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A195" s="2"/>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A196" s="3"/>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A197" s="2"/>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A200" s="3"/>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A201" s="3"/>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A202" s="2"/>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A203" s="3"/>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A204" s="2"/>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A207" s="3"/>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A208" s="3"/>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A209" s="2"/>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A210" s="3"/>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A211" s="2"/>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A214" s="3"/>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A215" s="3"/>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A216" s="2"/>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A217" s="3"/>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A218" s="2"/>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A221" s="3"/>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A222" s="3"/>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A223" s="2"/>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A224" s="3"/>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A225" s="2"/>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A228" s="3"/>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A229" s="3"/>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A230" s="2"/>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A231" s="3"/>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A232" s="2"/>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A235" s="3"/>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A236" s="3"/>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A237" s="2"/>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A238" s="3"/>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A239" s="2"/>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A242" s="3"/>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A243" s="3"/>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A244" s="2"/>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A245" s="3"/>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A246" s="2"/>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A249" s="3"/>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A250" s="3"/>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A251" s="2"/>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A252" s="3"/>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A253" s="2"/>
+    </row>
+    <row r="256" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A256" s="3"/>
+    </row>
+    <row r="257" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A257" s="3"/>
+    </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A258" s="2"/>
+    </row>
+    <row r="259" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A259" s="3"/>
+    </row>
+    <row r="260" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A260" s="2"/>
+    </row>
+    <row r="263" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A263" s="3"/>
+    </row>
+    <row r="264" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A264" s="3"/>
+    </row>
+    <row r="265" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A265" s="2"/>
+    </row>
+    <row r="266" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A266" s="3"/>
+    </row>
+    <row r="267" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A267" s="2"/>
+    </row>
+    <row r="270" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A270" s="3"/>
+    </row>
+    <row r="271" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A271" s="3"/>
+    </row>
+    <row r="272" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A272" s="2"/>
+    </row>
+    <row r="273" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A273" s="3"/>
+    </row>
+    <row r="274" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A274" s="2"/>
+    </row>
+    <row r="277" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A277" s="3"/>
+    </row>
+    <row r="278" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A278" s="3"/>
+    </row>
+    <row r="279" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A279" s="2"/>
+    </row>
+    <row r="280" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A280" s="3"/>
+    </row>
+    <row r="281" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A281" s="2"/>
+    </row>
+    <row r="284" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A284" s="3"/>
+    </row>
+    <row r="285" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A285" s="3"/>
+    </row>
+    <row r="286" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A286" s="2"/>
+    </row>
+    <row r="287" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A287" s="3"/>
+    </row>
+    <row r="288" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A288" s="2"/>
+    </row>
+    <row r="291" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A291" s="3"/>
+    </row>
+    <row r="292" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A292" s="3"/>
+    </row>
+    <row r="293" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A293" s="2"/>
+    </row>
+    <row r="294" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A294" s="3"/>
+    </row>
+    <row r="295" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A295" s="2"/>
+    </row>
+    <row r="298" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A298" s="3"/>
+    </row>
+    <row r="299" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A299" s="3"/>
+    </row>
+    <row r="300" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A300" s="2"/>
+    </row>
+    <row r="301" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A301" s="3"/>
+    </row>
+    <row r="302" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A302" s="2"/>
+    </row>
+    <row r="305" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A305" s="3"/>
+    </row>
+    <row r="306" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A306" s="3"/>
+    </row>
+    <row r="307" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A307" s="2"/>
+    </row>
+    <row r="308" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A308" s="3"/>
+    </row>
+    <row r="309" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A309" s="2"/>
+    </row>
+    <row r="312" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A312" s="3"/>
+    </row>
+    <row r="313" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A313" s="3"/>
+    </row>
+    <row r="314" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A314" s="2"/>
+    </row>
+    <row r="315" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A315" s="3"/>
+    </row>
+    <row r="316" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A316" s="2"/>
+    </row>
+    <row r="319" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A319" s="3"/>
+    </row>
+    <row r="320" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A320" s="3"/>
+    </row>
+    <row r="321" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A321" s="2"/>
+    </row>
+    <row r="322" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A322" s="3"/>
+    </row>
+    <row r="323" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A323" s="2"/>
+    </row>
+    <row r="324" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A324">
+        <v>2.085838253618149</v>
+      </c>
+    </row>
+    <row r="325" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A325" s="4">
+        <v>44693.668064490739</v>
+      </c>
+    </row>
+    <row r="326" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A326" s="4">
+        <v>44693.668088449071</v>
+      </c>
+    </row>
+    <row r="327" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A327" s="2">
+        <v>2.3958333333333331E-5</v>
+      </c>
+    </row>
+    <row r="328" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A328" s="4">
+        <v>44693.668089629631</v>
+      </c>
+    </row>
+    <row r="329" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A329" s="2">
+        <v>1.180555555555556E-6</v>
+      </c>
+    </row>
+    <row r="330" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A330">
+        <v>4.0111069998492468</v>
+      </c>
+    </row>
+    <row r="331" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A331" s="4">
+        <v>44693.668076562499</v>
+      </c>
+    </row>
+    <row r="332" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A332" s="4">
+        <v>44693.668115162043</v>
+      </c>
+    </row>
+    <row r="333" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A333" s="2">
+        <v>3.8599537037037027E-5</v>
+      </c>
+    </row>
+    <row r="334" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A334" s="4">
+        <v>44693.668118032409</v>
+      </c>
+    </row>
+    <row r="335" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A335" s="2">
+        <v>2.8703703703703702E-6</v>
+      </c>
+    </row>
+    <row r="336" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A336">
+        <v>3.9734351072095819</v>
+      </c>
+    </row>
+    <row r="337" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A337" s="4">
+        <v>44693.668088344908</v>
+      </c>
+    </row>
+    <row r="338" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A338" s="4">
+        <v>44693.668138611109</v>
+      </c>
+    </row>
+    <row r="339" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A339" s="2">
+        <v>5.0266203703703702E-5</v>
+      </c>
+    </row>
+    <row r="340" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A340" s="4">
+        <v>44693.668141249997</v>
+      </c>
+    </row>
+    <row r="341" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A341" s="2">
+        <v>2.6273148148148152E-6</v>
+      </c>
+    </row>
+    <row r="342" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A342">
+        <v>3.0728986764067372</v>
+      </c>
+    </row>
+    <row r="343" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A343" s="4">
+        <v>44693.6680996875</v>
+      </c>
+    </row>
+    <row r="344" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A344" s="4">
+        <v>44693.668156458327</v>
+      </c>
+    </row>
+    <row r="345" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A345" s="2">
+        <v>5.6770833333333342E-5</v>
+      </c>
+    </row>
+    <row r="346" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A346" s="4">
+        <v>44693.668158692133</v>
+      </c>
+    </row>
+    <row r="347" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A347" s="2">
+        <v>2.2222222222222221E-6</v>
+      </c>
+    </row>
+    <row r="348" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A348">
+        <v>3.0728986764067372</v>
+      </c>
+    </row>
+    <row r="349" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A349" s="4">
+        <v>44693.668111550927</v>
+      </c>
+    </row>
+    <row r="350" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A350" s="4">
+        <v>44693.668174004633</v>
+      </c>
+    </row>
+    <row r="351" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A351" s="2">
+        <v>6.24537037037037E-5</v>
+      </c>
+    </row>
+    <row r="352" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A352" s="4">
+        <v>44693.668176041669</v>
+      </c>
+    </row>
+    <row r="353" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A353" s="2">
+        <v>2.0486111111111112E-6</v>
+      </c>
+    </row>
+    <row r="354" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A354">
+        <v>2.7357211299149782</v>
+      </c>
+    </row>
+    <row r="355" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A355" s="4">
+        <v>44693.668123067131</v>
+      </c>
+    </row>
+    <row r="356" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A356" s="4">
+        <v>44693.668192407407</v>
+      </c>
+    </row>
+    <row r="357" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A357" s="2">
+        <v>6.9340277777777773E-5</v>
+      </c>
+    </row>
+    <row r="358" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A358" s="4">
+        <v>44693.668194085651</v>
+      </c>
+    </row>
+    <row r="359" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A359" s="2">
+        <v>1.678240740740741E-6</v>
+      </c>
+    </row>
+    <row r="360" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A360">
+        <v>2.710672863296594</v>
+      </c>
+    </row>
+    <row r="361" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A361" s="4">
+        <v>44693.66813474537</v>
+      </c>
+    </row>
+    <row r="362" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A362" s="4">
+        <v>44693.668210185177</v>
+      </c>
+    </row>
+    <row r="363" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A363" s="2">
+        <v>7.5439814814814816E-5</v>
+      </c>
+    </row>
+    <row r="364" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A364" s="4">
+        <v>44693.66821210648</v>
+      </c>
+    </row>
+    <row r="365" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A365" s="2">
+        <v>1.9328703703703699E-6</v>
+      </c>
+    </row>
+    <row r="366" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A366">
+        <v>2.7587354043616301</v>
+      </c>
+    </row>
+    <row r="367" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A367" s="4">
+        <v>44693.668146319447</v>
+      </c>
+    </row>
+    <row r="368" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A368" s="4">
+        <v>44693.668227387323</v>
+      </c>
+    </row>
+    <row r="369" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A369" s="2">
+        <v>8.1067870370370369E-5</v>
+      </c>
+    </row>
+    <row r="370" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A370" s="4">
+        <v>44693.668229280578</v>
+      </c>
+    </row>
+    <row r="371" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A371" s="2">
+        <v>1.8932638888888891E-6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>